<commit_message>
minor edit for refresh
</commit_message>
<xml_diff>
--- a/spec/test-sheet-1.xlsx
+++ b/spec/test-sheet-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcjadud/git/FAC/xlsx/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E351FB-DE88-A742-8F2B-AB355F7B0337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A13E6B-49D3-7044-8FFF-E7A88CBAEE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{DA1A9B60-C8C2-C54B-A827-41A908274057}"/>
+    <workbookView xWindow="260" yWindow="860" windowWidth="20520" windowHeight="14200" xr2:uid="{DA1A9B60-C8C2-C54B-A827-41A908274057}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Entry" sheetId="1" r:id="rId1"/>
@@ -382,20 +382,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC58C028-BA10-F84E-A24D-046B6CCF6569}">
-  <dimension ref="D2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D2">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>